<commit_message>
Cambios en iniciar sesionPruebas
</commit_message>
<xml_diff>
--- a/Entrega 4/Pruebas/GuardarExamen.xlsx
+++ b/Entrega 4/Pruebas/GuardarExamen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pepus Perez Flores\Documents\DAW2020\Entrega 4\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3052D6D-6784-45BF-A985-C76F5E029FE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5E6839-3D18-4BB7-B10E-6AFB938543FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Escenarios alternativos</t>
   </si>
@@ -40,6 +40,42 @@
   </si>
   <si>
     <t>Resultado Esperado</t>
+  </si>
+  <si>
+    <t>Todos los campos son llenados de forma correcta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El examen se almacena en el sistema </t>
+  </si>
+  <si>
+    <t>Numero preguntas invalido</t>
+  </si>
+  <si>
+    <t>Examen creado con éxito</t>
+  </si>
+  <si>
+    <t>Error: Numero de preguntas invalido</t>
+  </si>
+  <si>
+    <t>Se ingresa un numero invalido para el total de preguntas</t>
+  </si>
+  <si>
+    <t>Caracteres invalidos preguntas</t>
+  </si>
+  <si>
+    <t>Se ingresan caracteres especiales en el total de preguntas</t>
+  </si>
+  <si>
+    <t>Error: Ingresar un numero</t>
+  </si>
+  <si>
+    <t>Letras en numero de preguntas</t>
+  </si>
+  <si>
+    <t>Se escribren letas en el total de preguntas en vez de numeros</t>
+  </si>
+  <si>
+    <t>Error:Ingresar un numero</t>
   </si>
 </sst>
 </file>
@@ -110,9 +146,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -130,6 +163,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,7 +450,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -426,182 +462,224 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="4"/>
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="4"/>
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="4">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="4"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="4"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="4"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="4"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="4"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="4"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="4"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="4"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="5"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="4"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="4"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="4"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="4"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>